<commit_message>
Added custom notifications documents
</commit_message>
<xml_diff>
--- a/public/sample_uploads/valuations.xlsx
+++ b/public/sample_uploads/valuations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F560E5BB-53A3-4495-98F8-49C7000BBC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CC62D9-704F-4F7D-9EDD-22A0C8CCE12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -554,7 +554,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -603,7 +603,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
-        <v>43881</v>
+        <v>44247</v>
       </c>
       <c r="B3" s="2">
         <v>1000</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
-        <v>43881</v>
+        <v>44247</v>
       </c>
       <c r="B5" s="2">
         <v>2000</v>

</xml_diff>